<commit_message>
Add missing department to export data
</commit_message>
<xml_diff>
--- a/management/src/main/resources/RegionMeetings_template.xlsx
+++ b/management/src/main/resources/RegionMeetings_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="3915"/>
@@ -10,7 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -40,7 +39,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="N2")</t>
+jx:area(lastCell="O2")</t>
         </r>
       </text>
     </comment>
@@ -64,7 +63,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="data" var="record" lastCell="N2")</t>
+jx:each(items="data" var="record" lastCell="O2")</t>
         </r>
       </text>
     </comment>
@@ -73,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>${record.region}</t>
   </si>
@@ -157,12 +156,18 @@
   </si>
   <si>
     <t>${record.salesPersonFullName}</t>
+  </si>
+  <si>
+    <t>科室</t>
+  </si>
+  <si>
+    <t>${record.department}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -321,6 +326,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -356,6 +378,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -532,18 +571,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="14" width="18.5703125" customWidth="1"/>
+    <col min="1" max="15" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -557,37 +596,40 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -601,53 +643,56 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>24</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H3" s="1"/>
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="1"/>
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>